<commit_message>
Ajout dans le fichier Excel et ectra.
</commit_message>
<xml_diff>
--- a/Docs/Annexe 1 BanFlow V2.xlsx
+++ b/Docs/Annexe 1 BanFlow V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandromacbook/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandromacbook/Documents/GitHub/BankFlow-V2/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D259FCAE-5D3B-9A47-8C4F-ED33AFD0EF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25503052-72D1-C547-9476-370730DE14DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25600" xr2:uid="{18DE0A85-9C4E-2849-8C39-B837103E1B98}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="23600" xr2:uid="{18DE0A85-9C4E-2849-8C39-B837103E1B98}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Catégorie</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>Disponible pour les clients particuliers ou professionnels, souvent sur rendez-vous.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travail à réaliser : </t>
+  </si>
+  <si>
+    <t>Réaliser les routes de l'API Fastify.</t>
+  </si>
+  <si>
+    <t>Faire les tables avec MIKRO ORM.</t>
+  </si>
+  <si>
+    <t>Réaliser le protocole en JAVA.</t>
   </si>
 </sst>
 </file>
@@ -605,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E04B6D-A4F9-4142-ABB5-6C58EDDA2BCA}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -814,6 +826,26 @@
         <v>51</v>
       </c>
     </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>